<commit_message>
add default hit time
Former-commit-id: 482e651c6966ce7b735a0a78f05b1f4bb10c1072 [formerly 15b00289295d1b745a3e83293c37b5e6c80ac659]
Former-commit-id: e74533e10e24358b82e799317f95bb8fc2752b9e
</commit_message>
<xml_diff>
--- a/_Out/Server/NFDataCfg/Excel_Struct/Skill.xlsx
+++ b/_Out/Server/NFDataCfg/Excel_Struct/Skill.xlsx
@@ -1,25 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lvsheng.huang\Desktop\NoahGameFrame\trunk\_Out\Server\NFDataCfg\Excel_Struct\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19560" windowHeight="8460"/>
+    <workbookView windowWidth="19560" windowHeight="8460"/>
   </bookViews>
   <sheets>
     <sheet name="Property" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="144525"/>
+  <extLst/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73">
   <si>
     <t>Id</t>
   </si>
@@ -223,37 +219,43 @@
   </si>
   <si>
     <t>AtkDis</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>与目标最合适的攻击距离</t>
   </si>
   <si>
     <t>NeedTar</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>与目标最合适的攻击距离</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>是否必须有目标才能释放</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DefaultHitTime</t>
+  </si>
+  <si>
+    <t>缺省打击时间（本来应该打到但是物理没碰撞到或者其他原因）</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="12"/>
       <name val="宋体"/>
-      <family val="2"/>
       <charset val="134"/>
     </font>
   </fonts>
@@ -274,8 +276,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -287,19 +304,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="千位分隔" xfId="1" builtinId="3"/>
+    <cellStyle name="货币" xfId="2" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="3" builtinId="6"/>
+    <cellStyle name="百分比" xfId="4" builtinId="5"/>
+    <cellStyle name="货币[0]" xfId="5" builtinId="7"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -598,7 +610,6 @@
           </a:gdLst>
           <a:ahLst/>
           <a:cxnLst/>
-          <a:rect l="0" t="0" r="0" b="0"/>
           <a:pathLst>
             <a:path w="21600" h="21600"/>
           </a:pathLst>
@@ -631,14 +642,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="23.875" customWidth="1"/>
     <col min="2" max="2" width="8.25" customWidth="1"/>
@@ -651,7 +663,7 @@
     <col min="10" max="10" width="150.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -683,7 +695,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:10">
       <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
@@ -715,7 +727,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:10">
       <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
@@ -747,7 +759,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:10">
       <c r="A4" s="1" t="s">
         <v>16</v>
       </c>
@@ -779,7 +791,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:10">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
@@ -811,7 +823,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:10">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -843,7 +855,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:10">
       <c r="A7" s="1" t="s">
         <v>22</v>
       </c>
@@ -875,7 +887,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:10">
       <c r="A8" s="1" t="s">
         <v>24</v>
       </c>
@@ -907,7 +919,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:10">
       <c r="A9" s="1" t="s">
         <v>26</v>
       </c>
@@ -939,7 +951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:10">
       <c r="A10" s="1" t="s">
         <v>28</v>
       </c>
@@ -971,7 +983,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:10">
       <c r="A11" s="1" t="s">
         <v>30</v>
       </c>
@@ -1003,7 +1015,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:10">
       <c r="A12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1035,7 +1047,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:10">
       <c r="A13" s="1" t="s">
         <v>34</v>
       </c>
@@ -1067,7 +1079,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:10">
       <c r="A14" s="1" t="s">
         <v>36</v>
       </c>
@@ -1099,7 +1111,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:10">
       <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
@@ -1131,7 +1143,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:10">
       <c r="A16" s="1" t="s">
         <v>41</v>
       </c>
@@ -1163,7 +1175,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:10">
       <c r="A17" s="1" t="s">
         <v>43</v>
       </c>
@@ -1195,7 +1207,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:10">
       <c r="A18" s="1" t="s">
         <v>45</v>
       </c>
@@ -1227,7 +1239,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:10">
       <c r="A19" s="1" t="s">
         <v>47</v>
       </c>
@@ -1259,7 +1271,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:10">
       <c r="A20" s="1" t="s">
         <v>49</v>
       </c>
@@ -1291,7 +1303,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:10">
       <c r="A21" s="1" t="s">
         <v>51</v>
       </c>
@@ -1323,7 +1335,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:10">
       <c r="A22" s="1" t="s">
         <v>53</v>
       </c>
@@ -1355,7 +1367,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:10">
       <c r="A23" s="1" t="s">
         <v>55</v>
       </c>
@@ -1387,7 +1399,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:10">
       <c r="A24" s="1" t="s">
         <v>57</v>
       </c>
@@ -1419,7 +1431,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:10">
       <c r="A25" s="1" t="s">
         <v>59</v>
       </c>
@@ -1451,7 +1463,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:10">
       <c r="A26" s="1" t="s">
         <v>61</v>
       </c>
@@ -1483,7 +1495,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:10">
       <c r="A27" s="1" t="s">
         <v>63</v>
       </c>
@@ -1515,7 +1527,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:10">
       <c r="A28" s="1" t="s">
         <v>65</v>
       </c>
@@ -1547,7 +1559,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:10">
       <c r="A29" s="1" t="s">
         <v>67</v>
       </c>
@@ -1576,12 +1588,12 @@
         <v>12</v>
       </c>
       <c r="J29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10">
+      <c r="A30" s="1" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.15">
-      <c r="A30" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>11</v>
@@ -1611,16 +1623,47 @@
         <v>70</v>
       </c>
     </row>
+    <row r="31" spans="1:10">
+      <c r="A31" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C31" t="b">
+        <v>0</v>
+      </c>
+      <c r="D31" t="b">
+        <v>0</v>
+      </c>
+      <c r="E31" t="b">
+        <v>0</v>
+      </c>
+      <c r="F31" t="b">
+        <v>1</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="H31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F30 F31 F2:F29 F32:F1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
</xml_diff>